<commit_message>
DRY and Mininet File change
+Functions in testbed.sh
+added # of rules & %age packet dropped in Simple_Pkt.py - mininet file
</commit_message>
<xml_diff>
--- a/Documents/SDN Languages-Programs (Autosaved).xlsx
+++ b/Documents/SDN Languages-Programs (Autosaved).xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/baba/Desktop/Thesis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/baba/Desktop/Thesis/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="69">
   <si>
     <t>Language</t>
   </si>
@@ -405,34 +405,34 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -719,7 +719,7 @@
   <dimension ref="A1:Q32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -734,23 +734,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="47" x14ac:dyDescent="0.55000000000000004">
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
     </row>
     <row r="3" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C3" s="10" t="s">
@@ -777,7 +777,7 @@
       <c r="J3" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="L3" s="20" t="s">
+      <c r="L3" s="12" t="s">
         <v>12</v>
       </c>
       <c r="M3" s="8" t="s">
@@ -819,12 +819,12 @@
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
-      <c r="I5" s="22" t="s">
+      <c r="I5" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="J5" s="22"/>
-      <c r="K5" s="22"/>
-      <c r="L5" s="22"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="16"/>
       <c r="M5" s="5"/>
       <c r="N5" s="5"/>
       <c r="O5" s="5"/>
@@ -843,10 +843,10 @@
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
-      <c r="I6" s="22"/>
-      <c r="J6" s="22"/>
-      <c r="K6" s="22"/>
-      <c r="L6" s="22"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
       <c r="M6" s="5"/>
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
@@ -867,10 +867,10 @@
         <v>65</v>
       </c>
       <c r="H7" s="5"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="22"/>
-      <c r="K7" s="22"/>
-      <c r="L7" s="22"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16"/>
       <c r="M7" s="5"/>
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
@@ -889,10 +889,10 @@
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
-      <c r="I8" s="22"/>
-      <c r="J8" s="22"/>
-      <c r="K8" s="22"/>
-      <c r="L8" s="22"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="16"/>
       <c r="M8" s="5"/>
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
@@ -910,11 +910,11 @@
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="22"/>
-      <c r="J9" s="22"/>
-      <c r="K9" s="22"/>
-      <c r="L9" s="22"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16"/>
       <c r="M9" s="5"/>
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
@@ -922,7 +922,9 @@
       <c r="Q9" s="5"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A10" s="3"/>
+      <c r="A10" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
@@ -1363,418 +1365,418 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="19"/>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
+      <c r="A2" s="20"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
     </row>
     <row r="3" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
     </row>
     <row r="4" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="16"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
+      <c r="A4" s="18"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
     </row>
     <row r="5" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
     </row>
     <row r="6" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="16"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
+      <c r="A6" s="18"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
     </row>
     <row r="7" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="C7" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
     </row>
     <row r="8" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="16"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
+      <c r="A8" s="18"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
     </row>
     <row r="9" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
     </row>
     <row r="10" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="16"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
+      <c r="A10" s="18"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
     </row>
     <row r="11" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
     </row>
     <row r="12" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="16"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
+      <c r="A12" s="18"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="19"/>
     </row>
     <row r="13" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="16" t="s">
+      <c r="A13" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
     </row>
     <row r="14" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="16"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
+      <c r="A14" s="18"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="19"/>
     </row>
     <row r="15" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="16" t="s">
+      <c r="A15" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="C15" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="15"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19"/>
     </row>
     <row r="16" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="16"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
+      <c r="A16" s="18"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
     </row>
     <row r="17" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="16" t="s">
+      <c r="A17" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="B17" s="16" t="s">
+      <c r="B17" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="16" t="s">
+      <c r="C17" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="15"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19"/>
     </row>
     <row r="18" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="16"/>
-      <c r="B18" s="16"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="15"/>
+      <c r="A18" s="18"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="19"/>
     </row>
     <row r="19" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="16" t="s">
+      <c r="A19" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="B19" s="16" t="s">
+      <c r="B19" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="16" t="s">
+      <c r="C19" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="15"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="19"/>
     </row>
     <row r="20" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="16"/>
-      <c r="B20" s="16"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="15"/>
+      <c r="A20" s="18"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="19"/>
     </row>
     <row r="21" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="16" t="s">
+      <c r="A21" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="16" t="s">
+      <c r="B21" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="16" t="s">
+      <c r="C21" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="15"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="19"/>
     </row>
     <row r="22" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="16"/>
-      <c r="B22" s="16"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="15"/>
+      <c r="A22" s="18"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="19"/>
     </row>
     <row r="23" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="16" t="s">
+      <c r="A23" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="B23" s="16" t="s">
+      <c r="B23" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="16" t="s">
+      <c r="C23" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="D23" s="15"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="15"/>
-      <c r="H23" s="15"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="19"/>
     </row>
     <row r="24" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="16"/>
-      <c r="B24" s="16"/>
-      <c r="C24" s="16"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
+      <c r="A24" s="18"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="19"/>
     </row>
     <row r="25" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="16" t="s">
+      <c r="A25" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="B25" s="16" t="s">
+      <c r="B25" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="C25" s="16" t="s">
+      <c r="C25" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="15"/>
-      <c r="H25" s="15"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="19"/>
     </row>
     <row r="26" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="16"/>
-      <c r="B26" s="16"/>
-      <c r="C26" s="16"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="15"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="15"/>
-      <c r="H26" s="15"/>
+      <c r="A26" s="18"/>
+      <c r="B26" s="18"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="19"/>
     </row>
     <row r="27" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="14" t="s">
+      <c r="A27" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="B27" s="14" t="s">
+      <c r="B27" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="C27" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="D27" s="15"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="15"/>
-      <c r="G27" s="15"/>
-      <c r="H27" s="15"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="19"/>
     </row>
     <row r="28" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="14"/>
-      <c r="B28" s="14"/>
-      <c r="C28" s="14"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="15"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="15"/>
-      <c r="H28" s="15"/>
+      <c r="A28" s="22"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
     </row>
     <row r="29" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="14" t="s">
+      <c r="A29" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="B29" s="14" t="s">
+      <c r="B29" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="C29" s="14" t="s">
+      <c r="C29" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="D29" s="15"/>
-      <c r="E29" s="15"/>
-      <c r="F29" s="15"/>
-      <c r="G29" s="15"/>
-      <c r="H29" s="15"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="19"/>
     </row>
     <row r="30" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="14"/>
-      <c r="B30" s="14"/>
-      <c r="C30" s="14"/>
-      <c r="D30" s="15"/>
-      <c r="E30" s="15"/>
-      <c r="F30" s="15"/>
-      <c r="G30" s="15"/>
-      <c r="H30" s="15"/>
+      <c r="A30" s="22"/>
+      <c r="B30" s="22"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="19"/>
+      <c r="H30" s="19"/>
     </row>
     <row r="31" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="16" t="s">
+      <c r="A31" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="B31" s="16" t="s">
+      <c r="B31" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C31" s="16" t="s">
+      <c r="C31" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="D31" s="15"/>
-      <c r="E31" s="15"/>
-      <c r="F31" s="15"/>
-      <c r="G31" s="15"/>
-      <c r="H31" s="15"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="19"/>
+      <c r="H31" s="19"/>
     </row>
     <row r="32" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="16"/>
-      <c r="B32" s="16"/>
-      <c r="C32" s="16"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="15"/>
-      <c r="F32" s="15"/>
-      <c r="G32" s="15"/>
-      <c r="H32" s="15"/>
+      <c r="A32" s="18"/>
+      <c r="B32" s="18"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="19"/>
+      <c r="E32" s="19"/>
+      <c r="F32" s="19"/>
+      <c r="G32" s="19"/>
+      <c r="H32" s="19"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="s">
@@ -1868,6 +1870,118 @@
     </row>
   </sheetData>
   <mergeCells count="128">
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="G29:G30"/>
+    <mergeCell ref="H29:H30"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="G31:G32"/>
+    <mergeCell ref="H31:H32"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="G25:G26"/>
+    <mergeCell ref="H25:H26"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="G27:G28"/>
+    <mergeCell ref="H27:H28"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="H21:H22"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="G23:G24"/>
+    <mergeCell ref="H23:H24"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="H7:H8"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="H1:H2"/>
@@ -1884,118 +1998,6 @@
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="H3:H4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="G17:G18"/>
-    <mergeCell ref="H17:H18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="H19:H20"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="G21:G22"/>
-    <mergeCell ref="H21:H22"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="F23:F24"/>
-    <mergeCell ref="G23:G24"/>
-    <mergeCell ref="H23:H24"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="G25:G26"/>
-    <mergeCell ref="H25:H26"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="F27:F28"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="G27:G28"/>
-    <mergeCell ref="H27:H28"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="G29:G30"/>
-    <mergeCell ref="H29:H30"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="F31:F32"/>
-    <mergeCell ref="G31:G32"/>
-    <mergeCell ref="H31:H32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>